<commit_message>
fixed excel conversion script
</commit_message>
<xml_diff>
--- a/examples/table_annotation/output_file.xlsx
+++ b/examples/table_annotation/output_file.xlsx
@@ -671,7 +671,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>annotations/2-9606_0002f40-Vertebrata_aln_slice.html</t>
+          <t>conservation_analysis/annotations/2-9606_0002f40-Vertebrata_aln_slice.html</t>
         </is>
       </c>
       <c r="H4" t="n">
@@ -686,9 +686,14 @@
       <c r="K4" t="n">
         <v>-0.6280728891063256</v>
       </c>
-      <c r="L4" s="2" t="inlineStr">
+      <c r="L4" t="inlineStr">
         <is>
           <t>/home/jch/Documents/05-conservation_pipeline/examples/table_annotation/conservation_analysis/2-9606_0_002f40/2-9606_0_002f40.json</t>
+        </is>
+      </c>
+      <c r="M4" s="2" t="inlineStr">
+        <is>
+          <t>conservation_analysis/annotations/2-9606_0002f40-pairk_aln_needleman_lf5_rf5_edssmat50_multilevel_plot.png</t>
         </is>
       </c>
       <c r="N4" t="n">
@@ -720,7 +725,7 @@
       </c>
       <c r="U4" s="2" t="inlineStr">
         <is>
-          <t>annotations/2-9606_0002f40-Vertebrata_aln_slice.html</t>
+          <t>conservation_analysis/annotations/2-9606_0002f40-Vertebrata_aln_slice.html</t>
         </is>
       </c>
       <c r="V4" t="n">
@@ -735,14 +740,14 @@
       <c r="Y4" t="n">
         <v>-0.9076025074355883</v>
       </c>
-      <c r="Z4" s="2" t="inlineStr">
+      <c r="Z4" t="inlineStr">
         <is>
           <t>/home/jch/Documents/05-conservation_pipeline/examples/table_annotation/conservation_analysis/2-9606_0_002f40/2-9606_0_002f40.json</t>
         </is>
       </c>
       <c r="AA4" s="2" t="inlineStr">
         <is>
-          <t>annotations/2-9606_0002f40-aln_property_entropy_multilevel_plot.png</t>
+          <t>conservation_analysis/annotations/2-9606_0002f40-aln_property_entropy_multilevel_plot.png</t>
         </is>
       </c>
       <c r="AB4" t="n">
@@ -794,7 +799,7 @@
       </c>
       <c r="G5" s="2" t="inlineStr">
         <is>
-          <t>annotations/3-9606_0002f40-Vertebrata_aln_slice.html</t>
+          <t>conservation_analysis/annotations/3-9606_0002f40-Vertebrata_aln_slice.html</t>
         </is>
       </c>
       <c r="H5" t="n">
@@ -809,9 +814,14 @@
       <c r="K5" t="n">
         <v>0.2312397995312583</v>
       </c>
-      <c r="L5" s="2" t="inlineStr">
+      <c r="L5" t="inlineStr">
         <is>
           <t>/home/jch/Documents/05-conservation_pipeline/examples/table_annotation/conservation_analysis/3-9606_0_002f40/3-9606_0_002f40.json</t>
+        </is>
+      </c>
+      <c r="M5" s="2" t="inlineStr">
+        <is>
+          <t>conservation_analysis/annotations/3-9606_0002f40-pairk_aln_needleman_lf5_rf5_edssmat50_multilevel_plot.png</t>
         </is>
       </c>
       <c r="N5" t="n">
@@ -829,7 +839,7 @@
       </c>
       <c r="U5" s="2" t="inlineStr">
         <is>
-          <t>annotations/3-9606_0002f40-Vertebrata_aln_slice.html</t>
+          <t>conservation_analysis/annotations/3-9606_0002f40-Vertebrata_aln_slice.html</t>
         </is>
       </c>
       <c r="V5" t="n">
@@ -844,14 +854,14 @@
       <c r="Y5" t="n">
         <v>-0.8448505445597071</v>
       </c>
-      <c r="Z5" s="2" t="inlineStr">
+      <c r="Z5" t="inlineStr">
         <is>
           <t>/home/jch/Documents/05-conservation_pipeline/examples/table_annotation/conservation_analysis/3-9606_0_002f40/3-9606_0_002f40.json</t>
         </is>
       </c>
       <c r="AA5" s="2" t="inlineStr">
         <is>
-          <t>annotations/3-9606_0002f40-aln_property_entropy_multilevel_plot.png</t>
+          <t>conservation_analysis/annotations/3-9606_0002f40-aln_property_entropy_multilevel_plot.png</t>
         </is>
       </c>
       <c r="AB5" t="n">
@@ -941,15 +951,13 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G4" r:id="rId1"/>
-    <hyperlink ref="L4" r:id="rId2"/>
+    <hyperlink ref="M4" r:id="rId2"/>
     <hyperlink ref="U4" r:id="rId3"/>
-    <hyperlink ref="Z4" r:id="rId4"/>
-    <hyperlink ref="AA4" r:id="rId5"/>
-    <hyperlink ref="G5" r:id="rId6"/>
-    <hyperlink ref="L5" r:id="rId7"/>
-    <hyperlink ref="U5" r:id="rId8"/>
-    <hyperlink ref="Z5" r:id="rId9"/>
-    <hyperlink ref="AA5" r:id="rId10"/>
+    <hyperlink ref="AA4" r:id="rId4"/>
+    <hyperlink ref="G5" r:id="rId5"/>
+    <hyperlink ref="M5" r:id="rId6"/>
+    <hyperlink ref="U5" r:id="rId7"/>
+    <hyperlink ref="AA5" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>